<commit_message>
added in region and no longer write accessory name in column 4
</commit_message>
<xml_diff>
--- a/eqpImportTest1.xlsx
+++ b/eqpImportTest1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chrisp\Desktop\Chris' Files\Sherpa\pup2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40019_{DC359EF0-B16F-42D9-9C2B-5085E20E431C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC50BA-E1B1-4BE6-8AD2-C65F9316F5E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440"/>
+    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1651,7 +1643,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2151,12 +2143,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC9" sqref="AC9"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2165,7 +2157,7 @@
     <col min="2" max="2" width="13.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="56.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2174,7 +2166,7 @@
     <col min="11" max="11" width="13.88671875" style="1" customWidth="1"/>
     <col min="12" max="12" width="16.5546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="84.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="10.88671875" style="1" customWidth="1"/>
@@ -58390,13 +58382,13 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:J65536 V9:V65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:J65536 V9:V65536" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A65536" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Access,Model"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:U65536 X9:AB65536 AF9:BS65536 B9:C65536">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:U65536 X9:AB65536 AF9:BS65536 B9:C65536" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>IF(ISNUMBER(B9),TRUE,FALSE)</formula1>
     </dataValidation>
   </dataValidations>
@@ -58406,7 +58398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58418,7 +58410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>